<commit_message>
Auto update Excel data tu Admin
</commit_message>
<xml_diff>
--- a/filetiendo.xlsx
+++ b/filetiendo.xlsx
@@ -4770,15 +4770,15 @@
       </c>
       <c r="E5">
         <f>VLOOKUP(C5,GBOC!$E$7:$DG$29,$B$20,0)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F5">
         <f>IFERROR(E5/D5,0)</f>
-        <v>0.125</v>
+        <v>0.875</v>
       </c>
       <c r="G5">
         <f>D5-E5</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f>VLOOKUP(C5,'Giao CT'!$D$6:$S$20,4,0)</f>
@@ -4897,16 +4897,15 @@
         <v>4</v>
       </c>
       <c r="AK5">
-        <f>VLOOKUP(C5,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL5">
         <f>200%-IFERROR(AK5/AJ5,0)</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AM5">
         <f>MAX(AL5,0)</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AN5">
         <f>VLOOKUP(C5,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -4914,15 +4913,15 @@
       </c>
       <c r="AO5">
         <f>VLOOKUP(C5,GBOC!$E$7:$DG$29,$B$29,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP5">
         <f>200%-IFERROR(AO5/AN5,0)</f>
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="AQ5">
         <f>MAX(AP5,0)</f>
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="AR5">
         <v>0.97</v>
@@ -5131,16 +5130,15 @@
         <v>4</v>
       </c>
       <c r="AK6">
-        <f>VLOOKUP(C6,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AL6">
         <f>200%-IFERROR(AK6/AJ6,0)</f>
-        <v>2</v>
+        <v>-0.25</v>
       </c>
       <c r="AM6">
         <f>MAX(AL6,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN6">
         <f>VLOOKUP(C6,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -5365,7 +5363,6 @@
         <v>4</v>
       </c>
       <c r="AK7">
-        <f>VLOOKUP(C7,GBOC!$E$7:$DG$29,$B$28,0)</f>
         <v>0</v>
       </c>
       <c r="AL7">
@@ -5599,16 +5596,15 @@
         <v>4</v>
       </c>
       <c r="AK8">
-        <f>VLOOKUP(C8,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL8">
         <f>200%-IFERROR(AK8/AJ8,0)</f>
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="AM8">
         <f>MAX(AL8,0)</f>
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="AN8">
         <f>VLOOKUP(C8,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -5786,15 +5782,15 @@
       </c>
       <c r="Y9">
         <f>VLOOKUP(C9,GBOC!$E$7:$DG$29,$B$25,0)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Z9">
         <f>IFERROR(Y9/X9,0)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AA9">
         <f>X9-Y9</f>
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="AB9">
         <f>VLOOKUP(C9,'Giao CT'!$D$6:$S$20,9,0)</f>
@@ -5833,16 +5829,15 @@
         <v>3</v>
       </c>
       <c r="AK9">
-        <f>VLOOKUP(C9,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL9">
         <f>200%-IFERROR(AK9/AJ9,0)</f>
-        <v>2</v>
+        <v>0.33333333333333326</v>
       </c>
       <c r="AM9">
         <f>MAX(AL9,0)</f>
-        <v>2</v>
+        <v>0.33333333333333326</v>
       </c>
       <c r="AN9">
         <f>VLOOKUP(C9,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -6020,15 +6015,15 @@
       </c>
       <c r="Y10">
         <f>VLOOKUP(C10,GBOC!$E$7:$DG$29,$B$25,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z10">
         <f>IFERROR(Y10/X10,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA10">
         <f>X10-Y10</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB10">
         <f>VLOOKUP(C10,'Giao CT'!$D$6:$S$20,9,0)</f>
@@ -6067,16 +6062,15 @@
         <v>4</v>
       </c>
       <c r="AK10">
-        <f>VLOOKUP(C10,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL10">
         <f>200%-IFERROR(AK10/AJ10,0)</f>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="AM10">
         <f>MAX(AL10,0)</f>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="AN10">
         <f>VLOOKUP(C10,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -6301,16 +6295,15 @@
         <v>4</v>
       </c>
       <c r="AK11">
-        <f>VLOOKUP(C11,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AL11">
         <f>200%-IFERROR(AK11/AJ11,0)</f>
-        <v>2</v>
+        <v>-2.75</v>
       </c>
       <c r="AM11">
         <f>MAX(AL11,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN11">
         <f>VLOOKUP(C11,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -6504,15 +6497,15 @@
       </c>
       <c r="AC12">
         <f>VLOOKUP(C12,GBOC!$E$7:$DG$29,$B$26,0)</f>
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="AD12">
         <f>IFERROR(AC12/AB12,0)</f>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="AE12">
         <f>AB12-AC12</f>
-        <v>-18</v>
+        <v>-30</v>
       </c>
       <c r="AF12">
         <f>VLOOKUP(C12,'Giao CT'!$D$6:$S$20,10,0)</f>
@@ -6535,16 +6528,15 @@
         <v>4</v>
       </c>
       <c r="AK12">
-        <f>VLOOKUP(C12,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL12">
         <f>200%-IFERROR(AK12/AJ12,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM12">
         <f>MAX(AL12,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN12">
         <f>VLOOKUP(C12,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -6738,15 +6730,15 @@
       </c>
       <c r="AC13">
         <f>VLOOKUP(C13,GBOC!$E$7:$DG$29,$B$26,0)</f>
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="AD13">
         <f>IFERROR(AC13/AB13,0)</f>
-        <v>1.8</v>
+        <v>2.2</v>
       </c>
       <c r="AE13">
         <f>AB13-AC13</f>
-        <v>-24</v>
+        <v>-36</v>
       </c>
       <c r="AF13">
         <f>VLOOKUP(C13,'Giao CT'!$D$6:$S$20,10,0)</f>
@@ -6769,16 +6761,15 @@
         <v>4</v>
       </c>
       <c r="AK13">
-        <f>VLOOKUP(C13,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AL13">
         <f>200%-IFERROR(AK13/AJ13,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM13">
         <f>MAX(AL13,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN13">
         <f>VLOOKUP(C13,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -7003,16 +6994,15 @@
         <v>4</v>
       </c>
       <c r="AK14">
-        <f>VLOOKUP(C14,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL14">
         <f>200%-IFERROR(AK14/AJ14,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM14">
         <f>MAX(AL14,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN14">
         <f>VLOOKUP(C14,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -7222,31 +7212,30 @@
       </c>
       <c r="AG15">
         <f>VLOOKUP(C15,GBOC!$E$7:$DG$29,$B$27,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH15">
         <f>IFERROR(AG15/AF15,0)</f>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="AI15">
         <f>AF15-AG15</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AJ15">
         <f>VLOOKUP(C15,'Giao CT'!$D$6:$S$20,11,0)</f>
         <v>4</v>
       </c>
       <c r="AK15">
-        <f>VLOOKUP(C15,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL15">
         <f>200%-IFERROR(AK15/AJ15,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM15">
         <f>MAX(AL15,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN15">
         <f>VLOOKUP(C15,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -7424,15 +7413,15 @@
       </c>
       <c r="Y16">
         <f>VLOOKUP(C16,GBOC!$E$7:$DG$29,$B$25,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z16">
         <f>IFERROR(Y16/X16,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA16">
         <f>X16-Y16</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB16">
         <f>VLOOKUP(C16,'Giao CT'!$D$6:$S$20,9,0)</f>
@@ -7471,16 +7460,15 @@
         <v>4</v>
       </c>
       <c r="AK16">
-        <f>VLOOKUP(C16,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL16">
         <f>200%-IFERROR(AK16/AJ16,0)</f>
-        <v>2</v>
+        <v>-0.5</v>
       </c>
       <c r="AM16">
         <f>MAX(AL16,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN16">
         <f>VLOOKUP(C16,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -7658,15 +7646,15 @@
       </c>
       <c r="Y17">
         <f>VLOOKUP(C17,GBOC!$E$7:$DG$29,$B$25,0)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Z17">
         <f>IFERROR(Y17/X17,0)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AA17">
         <f>X17-Y17</f>
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="AB17">
         <f>VLOOKUP(C17,'Giao CT'!$D$6:$S$20,9,0)</f>
@@ -7705,16 +7693,15 @@
         <v>4</v>
       </c>
       <c r="AK17">
-        <f>VLOOKUP(C17,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL17">
         <f>200%-IFERROR(AK17/AJ17,0)</f>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="AM17">
         <f>MAX(AL17,0)</f>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="AN17">
         <f>VLOOKUP(C17,'Giao CT'!$D$6:$S$20,12,0)</f>
@@ -7939,16 +7926,15 @@
         <v>3</v>
       </c>
       <c r="AK18">
-        <f>VLOOKUP(C18,GBOC!$E$7:$DG$29,$B$28,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL18">
         <f>200%-IFERROR(AK18/AJ18,0)</f>
-        <v>2</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="AM18">
         <f>MAX(AL18,0)</f>
-        <v>2</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="AN18">
         <f>VLOOKUP(C18,'Giao CT'!$D$6:$S$20,12,0)</f>

</xml_diff>